<commit_message>
Removed test scripts and functions
</commit_message>
<xml_diff>
--- a/Medicaid-to-Medicare fee index by service type.xlsx
+++ b/Medicaid-to-Medicare fee index by service type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/263e6c96784ab765/Desktop/Common_Health/Measles_USA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{B808C449-86CA-4759-9310-196D895047CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33E7DF78-4296-429C-8763-45DC502E59F7}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{B808C449-86CA-4759-9310-196D895047CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1D3F39C-5E52-4861-85B9-F2EE421EC637}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D66AD839-7FD0-4A95-AE71-68BA29CB3155}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>Hawaii</t>
   </si>
   <si>
-    <t>Idahoa</t>
-  </si>
-  <si>
     <t>Illinois</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>Iowa</t>
   </si>
   <si>
-    <t>Kansasa</t>
-  </si>
-  <si>
     <t>Kentucky</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>Minnesota</t>
   </si>
   <si>
-    <t>Missouria</t>
-  </si>
-  <si>
     <t>Montana</t>
   </si>
   <si>
@@ -161,9 +152,6 @@
     <t>West Virginia</t>
   </si>
   <si>
-    <t>Wyominga</t>
-  </si>
-  <si>
     <t>Alabama</t>
   </si>
   <si>
@@ -203,7 +191,19 @@
     <t>District of Columbia</t>
   </si>
   <si>
-    <t>Tennessee </t>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
   </si>
 </sst>
 </file>
@@ -256,6 +256,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -577,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E7576C-40CC-4B35-815E-B03B6DA4ECEA}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +609,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>0.84</v>
@@ -741,7 +745,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B10">
         <v>0.57999999999999996</v>
@@ -758,7 +762,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B11">
         <v>0.83</v>
@@ -792,7 +796,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="B13">
         <v>0.93</v>
@@ -809,7 +813,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>0.59</v>
@@ -826,7 +830,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>0.77</v>
@@ -843,7 +847,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>0.81</v>
@@ -860,7 +864,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="B17">
         <v>0.71</v>
@@ -877,7 +881,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>0.76</v>
@@ -894,7 +898,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>0.69</v>
@@ -911,7 +915,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>0.66</v>
@@ -928,7 +932,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>0.9</v>
@@ -945,7 +949,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>0.78</v>
@@ -962,7 +966,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>0.69</v>
@@ -979,7 +983,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>0.74</v>
@@ -996,7 +1000,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B25">
         <v>0.92</v>
@@ -1013,7 +1017,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="B26">
         <v>0.62</v>
@@ -1030,7 +1034,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B27">
         <v>1.1100000000000001</v>
@@ -1047,7 +1051,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B28">
         <v>1.05</v>
@@ -1064,7 +1068,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B29">
         <v>0.96</v>
@@ -1081,7 +1085,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B30">
         <v>0.56999999999999995</v>
@@ -1098,7 +1102,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B31">
         <v>0.5</v>
@@ -1115,7 +1119,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B32">
         <v>0.93</v>
@@ -1132,7 +1136,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B33">
         <v>0.56999999999999995</v>
@@ -1149,7 +1153,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B34">
         <v>0.78</v>
@@ -1166,7 +1170,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1183,7 +1187,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B36">
         <v>0.62</v>
@@ -1200,7 +1204,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B37">
         <v>0.94</v>
@@ -1217,7 +1221,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B38">
         <v>0.83</v>
@@ -1234,7 +1238,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B39">
         <v>0.68</v>
@@ -1251,7 +1255,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B40">
         <v>0.37</v>
@@ -1268,7 +1272,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B41">
         <v>0.98</v>
@@ -1285,7 +1289,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B42">
         <v>0.85</v>
@@ -1302,7 +1306,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B43">
         <v>0.65</v>
@@ -1319,7 +1323,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B44">
         <v>0.81</v>
@@ -1336,7 +1340,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B45">
         <v>0.86</v>
@@ -1353,7 +1357,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B46">
         <v>0.78</v>
@@ -1370,7 +1374,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B47">
         <v>0.69</v>
@@ -1387,7 +1391,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B48">
         <v>0.8</v>
@@ -1404,7 +1408,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B49">
         <v>0.71</v>
@@ -1421,7 +1425,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B50">
         <v>0.62</v>
@@ -1438,7 +1442,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B51">
         <v>0.96</v>

</xml_diff>